<commit_message>
fix user full name in submissions
</commit_message>
<xml_diff>
--- a/LMS_API_School_Prj/LMS.API/UploadedSubmissions/test user registration.xlsx
+++ b/LMS_API_School_Prj/LMS.API/UploadedSubmissions/test user registration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0180C9B3-5888-46B6-98C4-3047833141DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDB5882-FB35-4823-B011-8DA0FB63A53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3720" yWindow="3225" windowWidth="26145" windowHeight="15345" xr2:uid="{B89E3CE8-29DE-48A4-9D77-060EF91A412B}"/>
   </bookViews>
@@ -89,7 +89,7 @@
     <t>Email</t>
   </si>
   <si>
-    <t>test@test.com</t>
+    <t>anasabualsoud@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -498,12 +498,12 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="4" max="4" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">

</xml_diff>